<commit_message>
updated test overview and fixed a bug in unicast schema.
</commit_message>
<xml_diff>
--- a/PlatformIndependentModeling/de.uni_paderborn.fujaba.muml.onetomanycommunicationschemata.synthesis/doc/TestOverview.xlsx
+++ b/PlatformIndependentModeling/de.uni_paderborn.fujaba.muml.onetomanycommunicationschemata.synthesis/doc/TestOverview.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="22">
   <si>
     <t>Unicast</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>LoadBalancing</t>
+  </si>
+  <si>
+    <t>UniReceive</t>
   </si>
 </sst>
 </file>
@@ -435,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -446,6 +455,7 @@
     <col min="4" max="4" width="21.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -579,6 +589,12 @@
       <c r="D15" t="s">
         <v>7</v>
       </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
@@ -649,6 +665,12 @@
       <c r="D20" t="s">
         <v>7</v>
       </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
@@ -662,6 +684,40 @@
       </c>
       <c r="D21" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:6">

</xml_diff>

<commit_message>
updated schema test list
</commit_message>
<xml_diff>
--- a/PlatformIndependentModeling/de.uni_paderborn.fujaba.muml.onetomanycommunicationschemata.synthesis/doc/TestOverview.xlsx
+++ b/PlatformIndependentModeling/de.uni_paderborn.fujaba.muml.onetomanycommunicationschemata.synthesis/doc/TestOverview.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="26">
   <si>
     <t>Unicast</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>memory exceedance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> correct</t>
   </si>
 </sst>
 </file>
@@ -611,7 +614,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -839,6 +842,13 @@
       <c r="D19" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="E19" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="22" t="s">
@@ -873,6 +883,12 @@
       <c r="D21" t="s">
         <v>5</v>
       </c>
+      <c r="E21" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="3" t="s">
@@ -887,6 +903,12 @@
       <c r="D22" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="E22" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
@@ -898,9 +920,16 @@
       <c r="C23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="D23" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="23"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
@@ -915,8 +944,12 @@
       <c r="D24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="E24" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>18</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
     <row r="26" spans="1:7">

</xml_diff>

<commit_message>
updated test results' overview
</commit_message>
<xml_diff>
--- a/PlatformIndependentModeling/de.uni_paderborn.fujaba.muml.onetomanycommunicationschemata.synthesis/doc/TestOverview.xlsx
+++ b/PlatformIndependentModeling/de.uni_paderborn.fujaba.muml.onetomanycommunicationschemata.synthesis/doc/TestOverview.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="26">
   <si>
     <t>Unicast</t>
   </si>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -1025,8 +1025,12 @@
       <c r="D29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7">
@@ -1042,8 +1046,12 @@
       <c r="D30" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">

</xml_diff>